<commit_message>
stil p bare miffed like init
</commit_message>
<xml_diff>
--- a/observeddata/Ebola_Incidence_Data_allempty.xlsx
+++ b/observeddata/Ebola_Incidence_Data_allempty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twhit957\Desktop\spatialEpisim\observeddata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1078C29C-6FA0-449D-8B55-3FA1EF470F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73C5BDD-050A-4856-80FA-62F5839D9577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Incidence" sheetId="1" r:id="rId1"/>
@@ -532,10 +532,10 @@
   <dimension ref="A1:AE1048"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE55" sqref="AE55"/>
+      <selection pane="bottomRight" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -677,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -863,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4" s="3">
         <v>0</v>
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3">
         <v>0</v>
@@ -1049,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6" s="3">
         <v>0</v>
@@ -1142,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E7" s="3">
         <v>0</v>
@@ -1235,7 +1235,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3">
         <v>0</v>
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
@@ -1421,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3">
         <v>0</v>
@@ -1514,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
@@ -1607,7 +1607,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E12" s="3">
         <v>0</v>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3">
         <v>0</v>
@@ -1793,7 +1793,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="3">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E14" s="3">
         <v>0</v>
@@ -1886,7 +1886,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E15" s="3">
         <v>0</v>
@@ -1979,7 +1979,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
@@ -2072,7 +2072,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="3">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
@@ -2165,7 +2165,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="3">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E18" s="3">
         <v>0</v>
@@ -2258,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="3">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E19" s="3">
         <v>0</v>
@@ -2351,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E20" s="3">
         <v>0</v>
@@ -2444,7 +2444,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E21" s="3">
         <v>0</v>
@@ -2537,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="3">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
@@ -2630,7 +2630,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="3">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E23" s="3">
         <v>0</v>
@@ -2723,7 +2723,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="3">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
@@ -2816,7 +2816,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="3">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
@@ -2909,7 +2909,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="3">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E26" s="3">
         <v>0</v>
@@ -3002,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="3">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E27" s="3">
         <v>0</v>
@@ -3095,7 +3095,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
@@ -3188,7 +3188,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="3">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="E29" s="3">
         <v>0</v>
@@ -3281,7 +3281,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="3">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
@@ -3374,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E31" s="3">
         <v>0</v>
@@ -3467,7 +3467,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="3">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E32" s="3">
         <v>0</v>
@@ -3560,7 +3560,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="3">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E33" s="3">
         <v>0</v>
@@ -3653,7 +3653,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="3">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="E34" s="3">
         <v>0</v>
@@ -3746,7 +3746,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="3">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E35" s="3">
         <v>0</v>
@@ -3839,7 +3839,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="3">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>
@@ -3932,7 +3932,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="3">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="E37" s="3">
         <v>0</v>
@@ -4025,7 +4025,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="3">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E38" s="3">
         <v>0</v>
@@ -4118,7 +4118,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="3">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E39" s="3">
         <v>0</v>
@@ -4211,7 +4211,7 @@
         <v>0</v>
       </c>
       <c r="D40" s="3">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="E40" s="3">
         <v>0</v>
@@ -4304,7 +4304,7 @@
         <v>0</v>
       </c>
       <c r="D41" s="3">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E41" s="3">
         <v>0</v>
@@ -4397,7 +4397,7 @@
         <v>0</v>
       </c>
       <c r="D42" s="3">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="E42" s="3">
         <v>0</v>
@@ -4490,7 +4490,7 @@
         <v>0</v>
       </c>
       <c r="D43" s="3">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="E43" s="3">
         <v>0</v>
@@ -4583,7 +4583,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="3">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="E44" s="3">
         <v>0</v>
@@ -4676,7 +4676,7 @@
         <v>0</v>
       </c>
       <c r="D45" s="3">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="E45" s="3">
         <v>0</v>
@@ -4769,7 +4769,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E46" s="3">
         <v>0</v>
@@ -4862,7 +4862,7 @@
         <v>0</v>
       </c>
       <c r="D47" s="3">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="E47" s="3">
         <v>0</v>
@@ -4955,7 +4955,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="3">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="E48" s="3">
         <v>0</v>
@@ -5048,7 +5048,7 @@
         <v>0</v>
       </c>
       <c r="D49" s="3">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E49" s="3">
         <v>0</v>

</xml_diff>